<commit_message>
some traces added and hume pipe raj kumar given and estiamte of subodh sir complete
</commit_message>
<xml_diff>
--- a/ofc/estimates/hume pipe raj kumar dai/as per ram mani sirह्युम पाइप बिछ्याउने कार्य.xlsx
+++ b/ofc/estimates/hume pipe raj kumar dai/as per ram mani sirह्युम पाइप बिछ्याउने कार्य.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4 (2)" sheetId="17" r:id="rId1"/>
@@ -360,7 +360,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -392,12 +392,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -541,46 +554,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,23 +587,45 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1169,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,113 +1204,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1367,14 +1383,14 @@
         <v>10</v>
       </c>
       <c r="E10" s="37">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F10" s="37">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G10" s="38">
         <f t="shared" ref="G10" si="0">PRODUCT(C10:F10)</f>
-        <v>3</v>
+        <v>3.0250000000000004</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
@@ -1399,7 +1415,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="33">
         <f>SUM(G10:G10)</f>
-        <v>3</v>
+        <v>3.0250000000000004</v>
       </c>
       <c r="H11" s="39" t="s">
         <v>44</v>
@@ -1409,7 +1425,7 @@
       </c>
       <c r="J11" s="43">
         <f>G11*I11</f>
-        <v>193.89</v>
+        <v>195.50575000000001</v>
       </c>
       <c r="K11" s="21"/>
       <c r="M11" s="25"/>
@@ -1434,7 +1450,7 @@
       <c r="I12" s="39"/>
       <c r="J12" s="43">
         <f>0.13*G11*19284/360</f>
-        <v>20.891000000000002</v>
+        <v>21.065091666666667</v>
       </c>
       <c r="K12" s="21"/>
       <c r="M12" s="25"/>
@@ -1636,7 +1652,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40">
         <f>SUM(J9:J18)</f>
-        <v>58130.299400000004</v>
+        <v>58132.089241666668</v>
       </c>
       <c r="K20" s="35"/>
     </row>
@@ -1658,14 +1674,12 @@
       <c r="B22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="72">
         <f>J20</f>
-        <v>58130.299400000004</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="38">
-        <v>100</v>
-      </c>
+        <v>58132.089241666668</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="E22" s="50"/>
       <c r="F22" s="49"/>
       <c r="G22" s="50"/>
       <c r="H22" s="49"/>
@@ -1673,16 +1687,16 @@
       <c r="J22" s="52"/>
       <c r="K22" s="53"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="54"/>
       <c r="B23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="80">
+      <c r="C23" s="75">
         <v>52000</v>
       </c>
-      <c r="D23" s="80"/>
-      <c r="E23" s="38"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="88"/>
       <c r="F23" s="47"/>
       <c r="G23" s="46"/>
       <c r="H23" s="46"/>
@@ -1690,19 +1704,19 @@
       <c r="J23" s="46"/>
       <c r="K23" s="47"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="54"/>
       <c r="B24" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="80">
+      <c r="C24" s="75">
         <f>C23-C26-C27</f>
         <v>49400</v>
       </c>
-      <c r="D24" s="80"/>
+      <c r="D24" s="75"/>
       <c r="E24" s="38">
         <f>C24/C22*100</f>
-        <v>84.981499338363975</v>
+        <v>84.978882824311313</v>
       </c>
       <c r="F24" s="47"/>
       <c r="G24" s="46"/>
@@ -1711,19 +1725,19 @@
       <c r="J24" s="46"/>
       <c r="K24" s="47"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54"/>
       <c r="B25" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="77">
+      <c r="C25" s="72">
         <f>C22-C24</f>
-        <v>8730.2994000000035</v>
-      </c>
-      <c r="D25" s="77"/>
+        <v>8732.0892416666684</v>
+      </c>
+      <c r="D25" s="72"/>
       <c r="E25" s="38">
         <f>100-E24</f>
-        <v>15.018500661636025</v>
+        <v>15.021117175688687</v>
       </c>
       <c r="F25" s="47"/>
       <c r="G25" s="46"/>
@@ -1732,16 +1746,16 @@
       <c r="J25" s="46"/>
       <c r="K25" s="47"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="54"/>
       <c r="B26" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="77">
+      <c r="C26" s="72">
         <f>C23*0.03</f>
         <v>1560</v>
       </c>
-      <c r="D26" s="77"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="38">
         <v>3</v>
       </c>
@@ -1752,1209 +1766,16 @@
       <c r="J26" s="46"/>
       <c r="K26" s="47"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="54"/>
       <c r="B27" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="77">
+      <c r="C27" s="72">
         <f>C23*0.02</f>
         <v>1040</v>
       </c>
-      <c r="D27" s="77"/>
-      <c r="E27" s="38">
-        <v>2</v>
-      </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="47"/>
-    </row>
-    <row r="28" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-    </row>
-    <row r="29" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-    </row>
-    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="71">
-        <f>F21</f>
-        <v>58130.299400000004</v>
-      </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="71">
-        <f>I21</f>
-        <v>57630.299400000004</v>
-      </c>
-      <c r="K6" s="72"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="I7" s="67" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="str">
-        <f>'Sheet4 (2)'!A6:F6</f>
-        <v xml:space="preserve">Project:- ह्युम पाइप बिछ्याउने कार्य </v>
-      </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="I8" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="69" t="str">
-        <f>'Sheet4 (2)'!A7:F7</f>
-        <v>Location:- Shankharapur Municipality 9</v>
-      </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="I9" s="68" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="63"/>
-      <c r="K12" s="64"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
-        <f>'Sheet4 (2)'!A9</f>
-        <v>1</v>
-      </c>
-      <c r="B13" s="32" t="str">
-        <f>'Sheet4 (2)'!B9</f>
-        <v>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Mechanical  Means ., Road way Excavation in  all types of soil as per Drawing and technical specifications  including  removal of stumps and other deleterious matter, all lifts and lead as per Drawing and instruction of the Engineer. (खन्ने पुर्ने )</v>
-      </c>
-      <c r="C13" s="12" t="str">
-        <f>'Sheet4 (2)'!H11</f>
-        <v>m3</v>
-      </c>
-      <c r="D13" s="12">
-        <f>'Sheet4 (2)'!G11</f>
-        <v>3</v>
-      </c>
-      <c r="E13" s="12">
-        <f>'Sheet4 (2)'!I11</f>
-        <v>64.63</v>
-      </c>
-      <c r="F13" s="12">
-        <f>D13*E13</f>
-        <v>193.89</v>
-      </c>
-      <c r="G13" s="12">
-        <f>V!G11</f>
-        <v>3</v>
-      </c>
-      <c r="H13" s="12">
-        <f>V!I11</f>
-        <v>64.63</v>
-      </c>
-      <c r="I13" s="12">
-        <f>G13*H13</f>
-        <v>193.89</v>
-      </c>
-      <c r="J13" s="28">
-        <f>I13-F13</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="14"/>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="85" t="str">
-        <f>'Sheet4 (2)'!B12</f>
-        <v>VAT calculation</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12">
-        <f>'Sheet4 (2)'!J12</f>
-        <v>20.891000000000002</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12">
-        <f>V!J12</f>
-        <v>20.891000000000002</v>
-      </c>
-      <c r="J14" s="28"/>
-      <c r="K14" s="14"/>
-    </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
-        <f>'Sheet4 (2)'!A14</f>
-        <v>2</v>
-      </c>
-      <c r="B16" s="32" t="str">
-        <f>'Sheet4 (2)'!B14</f>
-        <v>Providing and Laying Reinforced cement concrete NP3 Flush jointed pipe for culverts including fixing with cement mortar 1:2 as per Drawing and Technical Specifications., 450 mm  internal dia.</v>
-      </c>
-      <c r="C16" s="12" t="str">
-        <f>'Sheet4 (2)'!H15</f>
-        <v>rm</v>
-      </c>
-      <c r="D16" s="12">
-        <f>'Sheet4 (2)'!G15</f>
-        <v>10</v>
-      </c>
-      <c r="E16" s="12">
-        <f>'Sheet4 (2)'!I15</f>
-        <v>5144.96</v>
-      </c>
-      <c r="F16" s="12">
-        <f>D16*E16</f>
-        <v>51449.599999999999</v>
-      </c>
-      <c r="G16" s="12">
-        <f>V!G15</f>
-        <v>10</v>
-      </c>
-      <c r="H16" s="12">
-        <f>V!I15</f>
-        <v>5144.96</v>
-      </c>
-      <c r="I16" s="12">
-        <f>G16*H16</f>
-        <v>51449.599999999999</v>
-      </c>
-      <c r="J16" s="28">
-        <f>I16-F16</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="85" t="str">
-        <f>'Sheet4 (2)'!B15</f>
-        <v>Sub-total</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12">
-        <f>'Sheet4 (2)'!J16</f>
-        <v>5965.9183999999996</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12">
-        <f>V!J16</f>
-        <v>5965.9183999999996</v>
-      </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
-        <f>'Sheet4 (2)'!A18</f>
-        <v>3</v>
-      </c>
-      <c r="B19" s="31" t="str">
-        <f>'Sheet4 (2)'!B18</f>
-        <v>Information board (सुचना पाटि)</v>
-      </c>
-      <c r="C19" s="12" t="str">
-        <f>'Sheet4 (2)'!H18</f>
-        <v>no.</v>
-      </c>
-      <c r="D19" s="12">
-        <f>'Sheet4 (2)'!G18</f>
-        <v>1</v>
-      </c>
-      <c r="E19" s="12">
-        <f>'Sheet4 (2)'!I18</f>
-        <v>500</v>
-      </c>
-      <c r="F19" s="12">
-        <f>D19*E19</f>
-        <v>500</v>
-      </c>
-      <c r="G19" s="12">
-        <f>V!G18</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="12">
-        <f>V!I18</f>
-        <v>500</v>
-      </c>
-      <c r="I19" s="12">
-        <f>G19*H19</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="28">
-        <f>I19-F19</f>
-        <v>-500</v>
-      </c>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7">
-        <f>SUM(F13:F19)</f>
-        <v>58130.299400000004</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7">
-        <f>SUM(I13:I19)</f>
-        <v>57630.299400000004</v>
-      </c>
-      <c r="J21" s="13">
-        <f>I21-F21</f>
-        <v>-500</v>
-      </c>
-      <c r="K21" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter xml:space="preserve">&amp;LPrepared By:
-&amp;CChecked By:
-&amp;RApproved By:
-</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S84"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="81" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="79"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="165" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
-        <v>1</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="21"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="35">
-        <v>1</v>
-      </c>
-      <c r="D10" s="37">
-        <v>10</v>
-      </c>
-      <c r="E10" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="37">
-        <v>0.6</v>
-      </c>
-      <c r="G10" s="38">
-        <f t="shared" ref="G10" si="0">PRODUCT(C10:F10)</f>
-        <v>3</v>
-      </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="21"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-    </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="33">
-        <f>SUM(G10:G10)</f>
-        <v>3</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="39">
-        <v>64.63</v>
-      </c>
-      <c r="J11" s="43">
-        <f>G11*I11</f>
-        <v>193.89</v>
-      </c>
-      <c r="K11" s="21"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="43">
-        <f>0.13*G11*19284/360</f>
-        <v>20.891000000000002</v>
-      </c>
-      <c r="K12" s="21"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="21"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-    </row>
-    <row r="14" spans="1:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
-        <v>2</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="19">
-        <v>4</v>
-      </c>
-      <c r="D14" s="20">
-        <v>2.5</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="33">
-        <f>PRODUCT(C14:F14)</f>
-        <v>10</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="21"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="33">
-        <f>SUM(G14)</f>
-        <v>10</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="23">
-        <v>5144.96</v>
-      </c>
-      <c r="J15" s="33">
-        <f>G15*I15</f>
-        <v>51449.599999999999</v>
-      </c>
-      <c r="K15" s="21"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="43">
-        <f>0.13*G15*57364.6/12.5</f>
-        <v>5965.9183999999996</v>
-      </c>
-      <c r="K16" s="21"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="25"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="35"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <v>3</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="19">
-        <v>0</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="33">
-        <f t="shared" ref="G18" si="1">PRODUCT(C18:F18)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="23">
-        <v>500</v>
-      </c>
-      <c r="J18" s="33">
-        <f>G18*I18</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="21"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="21"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40">
-        <f>SUM(J9:J18)</f>
-        <v>57630.299400000004</v>
-      </c>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="56"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="55"/>
-    </row>
-    <row r="22" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="77">
-        <f>J20</f>
-        <v>57630.299400000004</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="38">
-        <v>100</v>
-      </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="53"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="80">
-        <v>52000</v>
-      </c>
-      <c r="D23" s="80"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="47"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="80">
-        <f>84.98%*C22</f>
-        <v>48974.228430120005</v>
-      </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="38">
-        <f>C24/C22*100</f>
-        <v>84.98</v>
-      </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="47"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="54"/>
-      <c r="B25" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="77">
-        <f>C22-C24</f>
-        <v>8656.0709698799983</v>
-      </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="38">
-        <f>100-E24</f>
-        <v>15.019999999999996</v>
-      </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="47"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="77">
-        <f>C23*0.03</f>
-        <v>1560</v>
-      </c>
-      <c r="D26" s="77"/>
-      <c r="E26" s="38">
-        <v>3</v>
-      </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="47"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="54"/>
-      <c r="B27" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="77">
-        <f>C23*0.02</f>
-        <v>1040</v>
-      </c>
-      <c r="D27" s="77"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="38">
         <v>2</v>
       </c>
@@ -3044,13 +1865,13 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -3060,12 +1881,503 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="76">
+        <f>F21</f>
+        <v>58132.089241666668</v>
+      </c>
+      <c r="D6" s="77"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="76">
+        <f>I21</f>
+        <v>57632.089241666668</v>
+      </c>
+      <c r="K6" s="77"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="I7" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="str">
+        <f>'Sheet4 (2)'!A6:F6</f>
+        <v xml:space="preserve">Project:- ह्युम पाइप बिछ्याउने कार्य </v>
+      </c>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="I8" s="85" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="86" t="str">
+        <f>'Sheet4 (2)'!A7:F7</f>
+        <v>Location:- Shankharapur Municipality 9</v>
+      </c>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="I9" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="81"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="81"/>
+      <c r="K12" s="82"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <f>'Sheet4 (2)'!A9</f>
+        <v>1</v>
+      </c>
+      <c r="B13" s="32" t="str">
+        <f>'Sheet4 (2)'!B9</f>
+        <v>Earthwork Excavation in Cutting., Roadway Excavation in all types of Soil by Mechanical  Means ., Road way Excavation in  all types of soil as per Drawing and technical specifications  including  removal of stumps and other deleterious matter, all lifts and lead as per Drawing and instruction of the Engineer. (खन्ने पुर्ने )</v>
+      </c>
+      <c r="C13" s="12" t="str">
+        <f>'Sheet4 (2)'!H11</f>
+        <v>m3</v>
+      </c>
+      <c r="D13" s="12">
+        <f>'Sheet4 (2)'!G11</f>
+        <v>3.0250000000000004</v>
+      </c>
+      <c r="E13" s="12">
+        <f>'Sheet4 (2)'!I11</f>
+        <v>64.63</v>
+      </c>
+      <c r="F13" s="12">
+        <f>D13*E13</f>
+        <v>195.50575000000001</v>
+      </c>
+      <c r="G13" s="12">
+        <f>V!G11</f>
+        <v>3.0250000000000004</v>
+      </c>
+      <c r="H13" s="12">
+        <f>V!I11</f>
+        <v>64.63</v>
+      </c>
+      <c r="I13" s="12">
+        <f>G13*H13</f>
+        <v>195.50575000000001</v>
+      </c>
+      <c r="J13" s="28">
+        <f>I13-F13</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+      <c r="B14" s="63" t="str">
+        <f>'Sheet4 (2)'!B12</f>
+        <v>VAT calculation</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12">
+        <f>'Sheet4 (2)'!J12</f>
+        <v>21.065091666666667</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12">
+        <f>V!J12</f>
+        <v>21.065091666666667</v>
+      </c>
+      <c r="J14" s="28"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <f>'Sheet4 (2)'!A14</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="32" t="str">
+        <f>'Sheet4 (2)'!B14</f>
+        <v>Providing and Laying Reinforced cement concrete NP3 Flush jointed pipe for culverts including fixing with cement mortar 1:2 as per Drawing and Technical Specifications., 450 mm  internal dia.</v>
+      </c>
+      <c r="C16" s="12" t="str">
+        <f>'Sheet4 (2)'!H15</f>
+        <v>rm</v>
+      </c>
+      <c r="D16" s="12">
+        <f>'Sheet4 (2)'!G15</f>
+        <v>10</v>
+      </c>
+      <c r="E16" s="12">
+        <f>'Sheet4 (2)'!I15</f>
+        <v>5144.96</v>
+      </c>
+      <c r="F16" s="12">
+        <f>D16*E16</f>
+        <v>51449.599999999999</v>
+      </c>
+      <c r="G16" s="12">
+        <f>V!G15</f>
+        <v>10</v>
+      </c>
+      <c r="H16" s="12">
+        <f>V!I15</f>
+        <v>5144.96</v>
+      </c>
+      <c r="I16" s="12">
+        <f>G16*H16</f>
+        <v>51449.599999999999</v>
+      </c>
+      <c r="J16" s="28">
+        <f>I16-F16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="14"/>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="63" t="str">
+        <f>'Sheet4 (2)'!B15</f>
+        <v>Sub-total</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12">
+        <f>'Sheet4 (2)'!J16</f>
+        <v>5965.9183999999996</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12">
+        <f>V!J16</f>
+        <v>5965.9183999999996</v>
+      </c>
+      <c r="J17" s="28"/>
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <f>'Sheet4 (2)'!A18</f>
+        <v>3</v>
+      </c>
+      <c r="B19" s="31" t="str">
+        <f>'Sheet4 (2)'!B18</f>
+        <v>Information board (सुचना पाटि)</v>
+      </c>
+      <c r="C19" s="12" t="str">
+        <f>'Sheet4 (2)'!H18</f>
+        <v>no.</v>
+      </c>
+      <c r="D19" s="12">
+        <f>'Sheet4 (2)'!G18</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="12">
+        <f>'Sheet4 (2)'!I18</f>
+        <v>500</v>
+      </c>
+      <c r="F19" s="12">
+        <f>D19*E19</f>
+        <v>500</v>
+      </c>
+      <c r="G19" s="12">
+        <f>V!G18</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
+        <f>V!I18</f>
+        <v>500</v>
+      </c>
+      <c r="I19" s="12">
+        <f>G19*H19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="28">
+        <f>I19-F19</f>
+        <v>-500</v>
+      </c>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7">
+        <f>SUM(F13:F19)</f>
+        <v>58132.089241666668</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7">
+        <f>SUM(I13:I19)</f>
+        <v>57632.089241666668</v>
+      </c>
+      <c r="J21" s="13">
+        <f>I21-F21</f>
+        <v>-500</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="85" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:
+&amp;RApproved By:
+</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S84"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,115 +2390,118 @@
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
+      <c r="A5" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="2"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="61" t="s">
+      <c r="H6" s="67" t="s">
         <v>40</v>
       </c>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="s">
+      <c r="A7" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
       <c r="G7" s="3"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="62" t="s">
+      <c r="H7" s="74" t="s">
         <v>50</v>
       </c>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -3259,14 +2574,14 @@
         <v>10</v>
       </c>
       <c r="E10" s="37">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F10" s="37">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G10" s="38">
         <f t="shared" ref="G10" si="0">PRODUCT(C10:F10)</f>
-        <v>3</v>
+        <v>3.0250000000000004</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="39"/>
@@ -3291,7 +2606,7 @@
       <c r="F11" s="37"/>
       <c r="G11" s="33">
         <f>SUM(G10:G10)</f>
-        <v>3</v>
+        <v>3.0250000000000004</v>
       </c>
       <c r="H11" s="39" t="s">
         <v>44</v>
@@ -3301,7 +2616,7 @@
       </c>
       <c r="J11" s="43">
         <f>G11*I11</f>
-        <v>193.89</v>
+        <v>195.50575000000001</v>
       </c>
       <c r="K11" s="21"/>
       <c r="M11" s="25"/>
@@ -3312,7 +2627,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="36" t="s">
         <v>38</v>
@@ -3326,7 +2641,7 @@
       <c r="I12" s="39"/>
       <c r="J12" s="43">
         <f>0.13*G11*19284/360</f>
-        <v>20.891000000000002</v>
+        <v>21.065091666666667</v>
       </c>
       <c r="K12" s="21"/>
       <c r="M12" s="25"/>
@@ -3372,7 +2687,7 @@
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="33">
+      <c r="G14" s="38">
         <f>PRODUCT(C14:F14)</f>
         <v>10</v>
       </c>
@@ -3420,7 +2735,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="36" t="s">
         <v>38</v>
@@ -3528,7 +2843,7 @@
       <c r="I20" s="40"/>
       <c r="J20" s="40">
         <f>SUM(J9:J18)</f>
-        <v>57630.299400000004</v>
+        <v>57632.089241666668</v>
       </c>
       <c r="K20" s="35"/>
     </row>
@@ -3545,19 +2860,17 @@
       <c r="J21" s="58"/>
       <c r="K21" s="55"/>
     </row>
-    <row r="22" spans="1:19" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="48"/>
       <c r="B22" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="72">
         <f>J20</f>
-        <v>57630.299400000004</v>
-      </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="38">
-        <v>100</v>
-      </c>
+        <v>57632.089241666668</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="E22" s="50"/>
       <c r="F22" s="49"/>
       <c r="G22" s="50"/>
       <c r="H22" s="49"/>
@@ -3570,10 +2883,710 @@
       <c r="B23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="80">
+      <c r="C23" s="75">
         <v>52000</v>
       </c>
-      <c r="D23" s="80"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="88">
+        <f>C24/C22*100</f>
+        <v>84.980000000000018</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="47"/>
+    </row>
+    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="54"/>
+      <c r="B24" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="75">
+        <f>84.98%*C22</f>
+        <v>48975.749437568338</v>
+      </c>
+      <c r="D24" s="75"/>
+      <c r="E24" s="38">
+        <f>100-E23</f>
+        <v>15.019999999999982</v>
+      </c>
+      <c r="F24" s="47"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="47"/>
+    </row>
+    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="54"/>
+      <c r="B25" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="72">
+        <f>C22-C24</f>
+        <v>8656.3398040983302</v>
+      </c>
+      <c r="D25" s="72"/>
+      <c r="E25" s="38">
+        <v>3</v>
+      </c>
+      <c r="F25" s="47"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="47"/>
+    </row>
+    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="54"/>
+      <c r="B26" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="72">
+        <f>C23*0.03</f>
+        <v>1560</v>
+      </c>
+      <c r="D26" s="72"/>
+      <c r="E26" s="38">
+        <v>2</v>
+      </c>
+      <c r="F26" s="47"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="47"/>
+    </row>
+    <row r="27" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="54"/>
+      <c r="B27" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="72">
+        <f>C23*0.02</f>
+        <v>1040</v>
+      </c>
+      <c r="D27" s="72"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="47"/>
+    </row>
+    <row r="28" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="55"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+    </row>
+    <row r="29" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:19" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E84"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S84"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="2"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="61" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="165" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>1</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="21"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="35">
+        <v>1</v>
+      </c>
+      <c r="D10" s="37">
+        <v>10</v>
+      </c>
+      <c r="E10" s="37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F10" s="37">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G10" s="38">
+        <f t="shared" ref="G10" si="0">PRODUCT(C10:F10)</f>
+        <v>3.0250000000000004</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="21"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="33">
+        <f>SUM(G10:G10)</f>
+        <v>3.0250000000000004</v>
+      </c>
+      <c r="H11" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" s="39">
+        <v>64.63</v>
+      </c>
+      <c r="J11" s="43">
+        <f>G11*I11</f>
+        <v>195.50575000000001</v>
+      </c>
+      <c r="K11" s="21"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+    </row>
+    <row r="12" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="43">
+        <f>0.13*G11*19284/360</f>
+        <v>21.065091666666667</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="21"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+    </row>
+    <row r="14" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>2</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="19">
+        <v>4</v>
+      </c>
+      <c r="D14" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="33">
+        <f>PRODUCT(C14:F14)</f>
+        <v>10</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="21"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="33">
+        <f>SUM(G14)</f>
+        <v>10</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="23">
+        <v>5144.96</v>
+      </c>
+      <c r="J15" s="33">
+        <f>G15*I15</f>
+        <v>51449.599999999999</v>
+      </c>
+      <c r="K15" s="21"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="35"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="43">
+        <f>0.13*G15*57364.6/12.5</f>
+        <v>5965.9183999999996</v>
+      </c>
+      <c r="K16" s="21"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="35"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>3</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="19">
+        <v>0</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="33">
+        <f t="shared" ref="G18" si="1">PRODUCT(C18:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="23">
+        <v>500</v>
+      </c>
+      <c r="J18" s="33">
+        <f>G18*I18</f>
+        <v>0</v>
+      </c>
+      <c r="K18" s="21"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="21"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="45"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40">
+        <f>SUM(J9:J18)</f>
+        <v>57632.089241666668</v>
+      </c>
+      <c r="K20" s="35"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="56"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="55"/>
+    </row>
+    <row r="22" spans="1:19" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="48"/>
+      <c r="B22" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="72">
+        <f>J20</f>
+        <v>57632.089241666668</v>
+      </c>
+      <c r="D22" s="72"/>
+      <c r="E22" s="38">
+        <v>100</v>
+      </c>
+      <c r="F22" s="49"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+    </row>
+    <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="54"/>
+      <c r="B23" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="75">
+        <v>52000</v>
+      </c>
+      <c r="D23" s="75"/>
       <c r="E23" s="38"/>
       <c r="F23" s="47"/>
       <c r="G23" s="46"/>
@@ -3587,14 +3600,14 @@
       <c r="B24" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="80">
+      <c r="C24" s="75">
         <f>84.98%*C22</f>
-        <v>48974.228430120005</v>
-      </c>
-      <c r="D24" s="80"/>
+        <v>48975.749437568338</v>
+      </c>
+      <c r="D24" s="75"/>
       <c r="E24" s="38">
         <f>C24/C22*100</f>
-        <v>84.98</v>
+        <v>84.980000000000018</v>
       </c>
       <c r="F24" s="47"/>
       <c r="G24" s="46"/>
@@ -3608,14 +3621,14 @@
       <c r="B25" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="77">
+      <c r="C25" s="72">
         <f>C22-C24</f>
-        <v>8656.0709698799983</v>
-      </c>
-      <c r="D25" s="77"/>
+        <v>8656.3398040983302</v>
+      </c>
+      <c r="D25" s="72"/>
       <c r="E25" s="38">
         <f>100-E24</f>
-        <v>15.019999999999996</v>
+        <v>15.019999999999982</v>
       </c>
       <c r="F25" s="47"/>
       <c r="G25" s="46"/>
@@ -3629,11 +3642,11 @@
       <c r="B26" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="77">
+      <c r="C26" s="72">
         <f>C23*0.03</f>
         <v>1560</v>
       </c>
-      <c r="D26" s="77"/>
+      <c r="D26" s="72"/>
       <c r="E26" s="38">
         <v>3</v>
       </c>
@@ -3649,11 +3662,11 @@
       <c r="B27" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="77">
+      <c r="C27" s="72">
         <f>C23*0.02</f>
         <v>1040</v>
       </c>
-      <c r="D27" s="77"/>
+      <c r="D27" s="72"/>
       <c r="E27" s="38">
         <v>2</v>
       </c>
@@ -3735,6 +3748,12 @@
     <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="A7:F7"/>
@@ -3742,12 +3761,6 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>